<commit_message>
Cucumber, ApachePOI day 11
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/Resources/ApacheExcel2.xlsx
+++ b/src/test/java/ApachePOI/Resources/ApacheExcel2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\Cucumber_Kursu4\src\test\java\ApachePOI\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragip\IdeaProjects\Us_Batch7_Cucumber\src\test\java\ApachePOI\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8595D97C-3C98-4BAF-9150-C494AAD4E4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="8970" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Lion</t>
   </si>
@@ -51,74 +52,68 @@
     <t>End</t>
   </si>
   <si>
-    <t>bir</t>
-  </si>
-  <si>
-    <t>iki</t>
-  </si>
-  <si>
-    <t>dort</t>
-  </si>
-  <si>
-    <t>bes</t>
-  </si>
-  <si>
-    <t>ulkemb3is111</t>
-  </si>
-  <si>
-    <t>ulkemb3is122</t>
-  </si>
-  <si>
-    <t>ulkemb3is133</t>
-  </si>
-  <si>
-    <t>ulkemb3is144</t>
-  </si>
-  <si>
-    <t>ulkemb3is155</t>
-  </si>
-  <si>
-    <t>ulkemb3is166</t>
-  </si>
-  <si>
-    <t>ulkemb3is177</t>
-  </si>
-  <si>
-    <t>ulkemb3is188</t>
-  </si>
-  <si>
-    <t>ub3is111</t>
-  </si>
-  <si>
-    <t>ub3is122</t>
-  </si>
-  <si>
-    <t>ub3is133</t>
-  </si>
-  <si>
-    <t>ub3is144</t>
-  </si>
-  <si>
-    <t>ub3is155</t>
-  </si>
-  <si>
-    <t>ub3is166</t>
-  </si>
-  <si>
-    <t>ub3is177</t>
-  </si>
-  <si>
-    <t>ub3is188</t>
+    <t>Us Batch 7 1</t>
+  </si>
+  <si>
+    <t>Us Batch 7 2</t>
+  </si>
+  <si>
+    <t>Us Batch 7 3</t>
+  </si>
+  <si>
+    <t>Us Batch 7 4</t>
+  </si>
+  <si>
+    <t>Us Batch 7 5</t>
+  </si>
+  <si>
+    <t>Us Batch 7 6</t>
+  </si>
+  <si>
+    <t>Us Batch 7 7</t>
+  </si>
+  <si>
+    <t>Us Batch 7 8</t>
+  </si>
+  <si>
+    <t>ub71</t>
+  </si>
+  <si>
+    <t>ub72</t>
+  </si>
+  <si>
+    <t>ub73</t>
+  </si>
+  <si>
+    <t>ub74</t>
+  </si>
+  <si>
+    <t>ub75</t>
+  </si>
+  <si>
+    <t>ub76</t>
+  </si>
+  <si>
+    <t>ub77</t>
+  </si>
+  <si>
+    <t>ub78</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -426,7 +421,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -509,11 +504,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B8"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,167 +516,72 @@
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>